<commit_message>
Cambios en la estructura de los gráficos y Anexo de Análisis de Supervisor y Contratistas
</commit_message>
<xml_diff>
--- a/BD_Rutas.xlsx
+++ b/BD_Rutas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fedbacks H1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEECB82-6E52-4E0A-91A1-840A06E47077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7BC1F5-FEDD-4190-A64E-E72F88BC551A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1434,13 +1434,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F77E348F-D8E6-4A65-830F-4E92A9C7A497}" name="Table2" displayName="Table2" ref="A1:F153" totalsRowShown="0">
-  <autoFilter ref="A1:F153" xr:uid="{F77E348F-D8E6-4A65-830F-4E92A9C7A497}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="CARLOS MUNGUIA"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F153" xr:uid="{F77E348F-D8E6-4A65-830F-4E92A9C7A497}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2116987D-B611-43E6-A00A-B1AAB9A17787}" name="RUTA"/>
     <tableColumn id="2" xr3:uid="{9B455927-9740-4DC5-818B-C0B4E45D2FFC}" name="CODIGO"/>
@@ -1719,7 +1713,7 @@
   <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E127"/>
+      <selection activeCell="D4" sqref="D4:D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1749,7 +1743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1769,7 +1763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1789,7 +1783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1809,7 +1803,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1829,7 +1823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1849,7 +1843,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1869,7 +1863,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1889,7 +1883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1909,7 +1903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1929,7 +1923,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1969,7 +1963,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -1989,7 +1983,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2009,7 +2003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2029,7 +2023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -2049,7 +2043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -2089,7 +2083,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>73</v>
       </c>
@@ -2109,7 +2103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -2129,7 +2123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -2149,7 +2143,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -2169,7 +2163,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -2186,7 +2180,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>87</v>
       </c>
@@ -2206,7 +2200,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -2226,7 +2220,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -2246,7 +2240,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>97</v>
       </c>
@@ -2266,7 +2260,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -2286,7 +2280,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -2306,7 +2300,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>106</v>
       </c>
@@ -2326,7 +2320,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>109</v>
       </c>
@@ -2346,7 +2340,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -2366,7 +2360,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -2386,7 +2380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>118</v>
       </c>
@@ -2406,7 +2400,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -2426,7 +2420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>124</v>
       </c>
@@ -2446,7 +2440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>127</v>
       </c>
@@ -2466,7 +2460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>130</v>
       </c>
@@ -2486,7 +2480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -2506,7 +2500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -2526,7 +2520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>139</v>
       </c>
@@ -2546,7 +2540,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>142</v>
       </c>
@@ -2560,7 +2554,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>144</v>
       </c>
@@ -2580,7 +2574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>147</v>
       </c>
@@ -2600,7 +2594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>150</v>
       </c>
@@ -2620,7 +2614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>153</v>
       </c>
@@ -2640,7 +2634,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>156</v>
       </c>
@@ -2660,7 +2654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>159</v>
       </c>
@@ -2680,7 +2674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>162</v>
       </c>
@@ -2697,7 +2691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>164</v>
       </c>
@@ -2717,7 +2711,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>168</v>
       </c>
@@ -2737,7 +2731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>171</v>
       </c>
@@ -2757,7 +2751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>174</v>
       </c>
@@ -2777,7 +2771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>177</v>
       </c>
@@ -2797,7 +2791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>180</v>
       </c>
@@ -2817,7 +2811,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>183</v>
       </c>
@@ -2837,7 +2831,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>186</v>
       </c>
@@ -2857,7 +2851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>189</v>
       </c>
@@ -2877,7 +2871,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>190</v>
       </c>
@@ -2897,7 +2891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>193</v>
       </c>
@@ -2917,7 +2911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>196</v>
       </c>
@@ -2937,7 +2931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>199</v>
       </c>
@@ -2957,7 +2951,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>202</v>
       </c>
@@ -2977,7 +2971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>205</v>
       </c>
@@ -2997,7 +2991,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>208</v>
       </c>
@@ -3017,7 +3011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>211</v>
       </c>
@@ -3057,7 +3051,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>217</v>
       </c>
@@ -3077,7 +3071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>220</v>
       </c>
@@ -3097,7 +3091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>223</v>
       </c>
@@ -3117,7 +3111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>226</v>
       </c>
@@ -3137,7 +3131,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>229</v>
       </c>
@@ -3157,7 +3151,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>232</v>
       </c>
@@ -3177,7 +3171,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>235</v>
       </c>
@@ -3197,7 +3191,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>238</v>
       </c>
@@ -3217,7 +3211,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>241</v>
       </c>
@@ -3237,7 +3231,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>244</v>
       </c>
@@ -3257,7 +3251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>247</v>
       </c>
@@ -3277,7 +3271,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>250</v>
       </c>
@@ -3297,7 +3291,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>253</v>
       </c>
@@ -3317,7 +3311,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>257</v>
       </c>
@@ -3337,7 +3331,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>260</v>
       </c>
@@ -3357,7 +3351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>263</v>
       </c>
@@ -3377,7 +3371,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>266</v>
       </c>
@@ -3397,7 +3391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>269</v>
       </c>
@@ -3417,7 +3411,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>272</v>
       </c>
@@ -3437,7 +3431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>275</v>
       </c>
@@ -3457,7 +3451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>278</v>
       </c>
@@ -3477,7 +3471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>281</v>
       </c>
@@ -3497,7 +3491,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>284</v>
       </c>
@@ -3517,7 +3511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>287</v>
       </c>
@@ -3537,7 +3531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>290</v>
       </c>
@@ -3557,7 +3551,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>293</v>
       </c>
@@ -3577,7 +3571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>296</v>
       </c>
@@ -3597,7 +3591,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>299</v>
       </c>
@@ -3617,7 +3611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>302</v>
       </c>
@@ -3637,7 +3631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>305</v>
       </c>
@@ -3657,7 +3651,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>308</v>
       </c>
@@ -3677,7 +3671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>311</v>
       </c>
@@ -3697,7 +3691,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>314</v>
       </c>
@@ -3717,7 +3711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>317</v>
       </c>
@@ -3737,7 +3731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>320</v>
       </c>
@@ -3757,7 +3751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>323</v>
       </c>
@@ -3777,7 +3771,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>326</v>
       </c>
@@ -3797,7 +3791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>329</v>
       </c>
@@ -3817,7 +3811,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>332</v>
       </c>
@@ -3837,7 +3831,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>335</v>
       </c>
@@ -3854,7 +3848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>338</v>
       </c>
@@ -3871,7 +3865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>340</v>
       </c>
@@ -3888,7 +3882,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>342</v>
       </c>
@@ -3905,7 +3899,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>344</v>
       </c>
@@ -3922,7 +3916,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>346</v>
       </c>
@@ -3942,7 +3936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>348</v>
       </c>
@@ -3962,7 +3956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>351</v>
       </c>
@@ -3979,7 +3973,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>353</v>
       </c>
@@ -3996,7 +3990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>355</v>
       </c>
@@ -4013,7 +4007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>357</v>
       </c>
@@ -4033,7 +4027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>360</v>
       </c>
@@ -4053,7 +4047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>363</v>
       </c>
@@ -4070,7 +4064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>365</v>
       </c>
@@ -4087,7 +4081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>367</v>
       </c>
@@ -4104,7 +4098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>369</v>
       </c>
@@ -4121,7 +4115,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>371</v>
       </c>
@@ -4138,7 +4132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>373</v>
       </c>
@@ -4155,7 +4149,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>375</v>
       </c>
@@ -4215,7 +4209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>384</v>
       </c>
@@ -4232,7 +4226,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>385</v>
       </c>
@@ -4252,7 +4246,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>388</v>
       </c>
@@ -4272,7 +4266,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>391</v>
       </c>
@@ -4292,7 +4286,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>394</v>
       </c>
@@ -4312,7 +4306,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>397</v>
       </c>
@@ -4332,7 +4326,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>400</v>
       </c>
@@ -4352,7 +4346,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>403</v>
       </c>
@@ -4372,7 +4366,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>406</v>
       </c>
@@ -4392,7 +4386,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>409</v>
       </c>
@@ -4412,7 +4406,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>412</v>
       </c>
@@ -4429,7 +4423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>414</v>
       </c>
@@ -4446,7 +4440,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>416</v>
       </c>
@@ -4466,7 +4460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>420</v>
       </c>
@@ -4486,7 +4480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>423</v>
       </c>
@@ -4506,7 +4500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>426</v>
       </c>
@@ -4526,7 +4520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>429</v>
       </c>
@@ -4543,7 +4537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>431</v>
       </c>
@@ -4563,7 +4557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>434</v>
       </c>
@@ -4580,7 +4574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>436</v>
       </c>
@@ -4597,7 +4591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>438</v>
       </c>
@@ -4617,7 +4611,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>441</v>
       </c>
@@ -4637,7 +4631,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>351</v>
       </c>
@@ -4654,7 +4648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>445</v>
       </c>
@@ -4671,7 +4665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>447</v>
       </c>
@@ -4688,7 +4682,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>449</v>
       </c>

</xml_diff>

<commit_message>
Análisis completo de Supervisores y mejoras visuales en general
</commit_message>
<xml_diff>
--- a/BD_Rutas.xlsx
+++ b/BD_Rutas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Fedbacks H1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7BC1F5-FEDD-4190-A64E-E72F88BC551A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC75F94-BC85-4293-8B4B-332C119B8976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1384,8 +1384,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1413,13 +1421,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1436,7 +1451,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F77E348F-D8E6-4A65-830F-4E92A9C7A497}" name="Table2" displayName="Table2" ref="A1:F153" totalsRowShown="0">
   <autoFilter ref="A1:F153" xr:uid="{F77E348F-D8E6-4A65-830F-4E92A9C7A497}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2116987D-B611-43E6-A00A-B1AAB9A17787}" name="RUTA"/>
+    <tableColumn id="1" xr3:uid="{2116987D-B611-43E6-A00A-B1AAB9A17787}" name="RUTA" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{9B455927-9740-4DC5-818B-C0B4E45D2FFC}" name="CODIGO"/>
     <tableColumn id="3" xr3:uid="{7AD54620-5CBF-4CE6-85B0-CACD6A1B8802}" name="PLACA"/>
     <tableColumn id="4" xr3:uid="{4BC9AA7B-C5FF-4931-A398-E7C37D480B20}" name="SUPERVISOR"/>
@@ -1713,7 +1728,7 @@
   <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D142"/>
+      <selection activeCell="A2" sqref="A2:A153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1744,7 +1759,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -1764,7 +1779,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
@@ -1784,7 +1799,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
@@ -1804,7 +1819,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
@@ -1824,7 +1839,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B6" t="s">
@@ -1844,7 +1859,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B7" t="s">
@@ -1864,7 +1879,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B8" t="s">
@@ -1884,7 +1899,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B9" t="s">
@@ -1904,7 +1919,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B10" t="s">
@@ -1924,7 +1939,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" t="s">
@@ -1944,7 +1959,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B12" t="s">
@@ -1964,7 +1979,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
@@ -1984,7 +1999,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B14" t="s">
@@ -2004,7 +2019,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B15" t="s">
@@ -2024,7 +2039,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B16" t="s">
@@ -2044,7 +2059,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B17" t="s">
@@ -2064,7 +2079,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B18" t="s">
@@ -2084,7 +2099,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B19" t="s">
@@ -2104,7 +2119,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B20" t="s">
@@ -2124,7 +2139,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B21" t="s">
@@ -2144,7 +2159,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B22" t="s">
@@ -2164,7 +2179,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B23" t="s">
@@ -2181,7 +2196,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B24" t="s">
@@ -2201,7 +2216,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B25" t="s">
@@ -2221,7 +2236,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B26" t="s">
@@ -2241,7 +2256,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B27" t="s">
@@ -2261,7 +2276,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B28" t="s">
@@ -2281,7 +2296,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B29" t="s">
@@ -2301,7 +2316,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B30" t="s">
@@ -2321,7 +2336,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B31" t="s">
@@ -2341,7 +2356,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B32" t="s">
@@ -2361,7 +2376,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B33" t="s">
@@ -2381,7 +2396,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B34" t="s">
@@ -2401,7 +2416,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B35" t="s">
@@ -2421,7 +2436,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B36" t="s">
@@ -2441,7 +2456,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B37" t="s">
@@ -2461,7 +2476,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B38" t="s">
@@ -2481,7 +2496,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>133</v>
       </c>
       <c r="B39" t="s">
@@ -2501,7 +2516,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B40" t="s">
@@ -2521,7 +2536,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B41" t="s">
@@ -2541,7 +2556,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B42" t="s">
@@ -2555,7 +2570,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B43" t="s">
@@ -2575,7 +2590,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>147</v>
       </c>
       <c r="B44" t="s">
@@ -2595,7 +2610,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B45" t="s">
@@ -2615,7 +2630,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B46" t="s">
@@ -2635,7 +2650,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>156</v>
       </c>
       <c r="B47" t="s">
@@ -2655,7 +2670,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B48" t="s">
@@ -2675,7 +2690,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>162</v>
       </c>
       <c r="C49" t="s">
@@ -2692,7 +2707,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B50" t="s">
@@ -2712,7 +2727,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B51" t="s">
@@ -2732,7 +2747,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B52" t="s">
@@ -2752,7 +2767,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>174</v>
       </c>
       <c r="B53" t="s">
@@ -2772,7 +2787,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>177</v>
       </c>
       <c r="B54" t="s">
@@ -2792,7 +2807,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B55" t="s">
@@ -2812,7 +2827,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>183</v>
       </c>
       <c r="B56" t="s">
@@ -2832,7 +2847,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B57" t="s">
@@ -2852,7 +2867,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>189</v>
       </c>
       <c r="B58" t="s">
@@ -2872,7 +2887,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>190</v>
       </c>
       <c r="B59" t="s">
@@ -2892,7 +2907,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>193</v>
       </c>
       <c r="B60" t="s">
@@ -2912,7 +2927,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B61" t="s">
@@ -2932,7 +2947,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>199</v>
       </c>
       <c r="B62" t="s">
@@ -2952,7 +2967,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B63" t="s">
@@ -2972,7 +2987,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>205</v>
       </c>
       <c r="B64" t="s">
@@ -2992,7 +3007,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B65" t="s">
@@ -3012,7 +3027,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>211</v>
       </c>
       <c r="B66" t="s">
@@ -3032,7 +3047,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+      <c r="A67" s="1" t="s">
         <v>214</v>
       </c>
       <c r="B67" t="s">
@@ -3052,7 +3067,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>217</v>
       </c>
       <c r="B68" t="s">
@@ -3072,7 +3087,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+      <c r="A69" s="1" t="s">
         <v>220</v>
       </c>
       <c r="B69" t="s">
@@ -3092,7 +3107,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+      <c r="A70" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B70" t="s">
@@ -3112,7 +3127,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>226</v>
       </c>
       <c r="B71" t="s">
@@ -3132,7 +3147,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>229</v>
       </c>
       <c r="B72" t="s">
@@ -3152,7 +3167,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>232</v>
       </c>
       <c r="B73" t="s">
@@ -3172,7 +3187,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+      <c r="A74" s="1" t="s">
         <v>235</v>
       </c>
       <c r="B74" t="s">
@@ -3192,7 +3207,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+      <c r="A75" s="1" t="s">
         <v>238</v>
       </c>
       <c r="B75" t="s">
@@ -3212,7 +3227,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>241</v>
       </c>
       <c r="B76" t="s">
@@ -3232,7 +3247,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+      <c r="A77" s="1" t="s">
         <v>244</v>
       </c>
       <c r="B77" t="s">
@@ -3252,7 +3267,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+      <c r="A78" s="1" t="s">
         <v>247</v>
       </c>
       <c r="B78" t="s">
@@ -3272,7 +3287,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+      <c r="A79" s="1" t="s">
         <v>250</v>
       </c>
       <c r="B79" t="s">
@@ -3292,7 +3307,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+      <c r="A80" s="1" t="s">
         <v>253</v>
       </c>
       <c r="B80" t="s">
@@ -3312,7 +3327,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+      <c r="A81" s="1" t="s">
         <v>257</v>
       </c>
       <c r="B81" t="s">
@@ -3332,7 +3347,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+      <c r="A82" s="1" t="s">
         <v>260</v>
       </c>
       <c r="B82" t="s">
@@ -3352,7 +3367,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+      <c r="A83" s="1" t="s">
         <v>263</v>
       </c>
       <c r="B83" t="s">
@@ -3372,7 +3387,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+      <c r="A84" s="1" t="s">
         <v>266</v>
       </c>
       <c r="B84" t="s">
@@ -3392,7 +3407,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+      <c r="A85" s="1" t="s">
         <v>269</v>
       </c>
       <c r="B85" t="s">
@@ -3412,7 +3427,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+      <c r="A86" s="1" t="s">
         <v>272</v>
       </c>
       <c r="B86" t="s">
@@ -3432,7 +3447,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+      <c r="A87" s="1" t="s">
         <v>275</v>
       </c>
       <c r="B87" t="s">
@@ -3452,7 +3467,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>278</v>
       </c>
       <c r="B88" t="s">
@@ -3472,7 +3487,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+      <c r="A89" s="1" t="s">
         <v>281</v>
       </c>
       <c r="B89" t="s">
@@ -3492,7 +3507,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+      <c r="A90" s="1" t="s">
         <v>284</v>
       </c>
       <c r="B90" t="s">
@@ -3512,7 +3527,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+      <c r="A91" s="1" t="s">
         <v>287</v>
       </c>
       <c r="B91" t="s">
@@ -3532,7 +3547,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+      <c r="A92" s="1" t="s">
         <v>290</v>
       </c>
       <c r="B92" t="s">
@@ -3552,7 +3567,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>293</v>
       </c>
       <c r="B93" t="s">
@@ -3572,7 +3587,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>296</v>
       </c>
       <c r="B94" t="s">
@@ -3592,7 +3607,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+      <c r="A95" s="1" t="s">
         <v>299</v>
       </c>
       <c r="B95" t="s">
@@ -3612,7 +3627,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+      <c r="A96" s="1" t="s">
         <v>302</v>
       </c>
       <c r="B96" t="s">
@@ -3632,7 +3647,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+      <c r="A97" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B97" t="s">
@@ -3652,7 +3667,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>308</v>
       </c>
       <c r="B98" t="s">
@@ -3672,7 +3687,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>311</v>
       </c>
       <c r="B99" t="s">
@@ -3692,7 +3707,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>314</v>
       </c>
       <c r="B100" t="s">
@@ -3712,7 +3727,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+      <c r="A101" s="1" t="s">
         <v>317</v>
       </c>
       <c r="B101" t="s">
@@ -3732,7 +3747,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+      <c r="A102" s="1" t="s">
         <v>320</v>
       </c>
       <c r="B102" t="s">
@@ -3752,7 +3767,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+      <c r="A103" s="1" t="s">
         <v>323</v>
       </c>
       <c r="B103" t="s">
@@ -3772,7 +3787,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+      <c r="A104" s="1" t="s">
         <v>326</v>
       </c>
       <c r="B104" t="s">
@@ -3792,7 +3807,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+      <c r="A105" s="1" t="s">
         <v>329</v>
       </c>
       <c r="B105" t="s">
@@ -3812,7 +3827,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+      <c r="A106" s="1" t="s">
         <v>332</v>
       </c>
       <c r="B106" t="s">
@@ -3832,7 +3847,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>335</v>
       </c>
       <c r="B107" t="s">
@@ -3849,7 +3864,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+      <c r="A108" s="1" t="s">
         <v>338</v>
       </c>
       <c r="B108" t="s">
@@ -3866,7 +3881,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+      <c r="A109" s="1" t="s">
         <v>340</v>
       </c>
       <c r="B109" t="s">
@@ -3883,7 +3898,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+      <c r="A110" s="1" t="s">
         <v>342</v>
       </c>
       <c r="B110" t="s">
@@ -3900,7 +3915,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>344</v>
       </c>
       <c r="B111" t="s">
@@ -3917,7 +3932,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+      <c r="A112" s="1" t="s">
         <v>346</v>
       </c>
       <c r="B112" t="s">
@@ -3937,7 +3952,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
+      <c r="A113" s="1" t="s">
         <v>348</v>
       </c>
       <c r="B113" t="s">
@@ -3957,7 +3972,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+      <c r="A114" s="1" t="s">
         <v>351</v>
       </c>
       <c r="B114" t="s">
@@ -3974,7 +3989,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+      <c r="A115" s="1" t="s">
         <v>353</v>
       </c>
       <c r="B115" t="s">
@@ -3991,7 +4006,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>355</v>
       </c>
       <c r="B116" t="s">
@@ -4008,7 +4023,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+      <c r="A117" s="1" t="s">
         <v>357</v>
       </c>
       <c r="B117" t="s">
@@ -4028,7 +4043,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+      <c r="A118" s="1" t="s">
         <v>360</v>
       </c>
       <c r="B118" t="s">
@@ -4048,7 +4063,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>363</v>
       </c>
       <c r="B119" t="s">
@@ -4065,7 +4080,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>365</v>
       </c>
       <c r="B120" t="s">
@@ -4082,7 +4097,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+      <c r="A121" s="1" t="s">
         <v>367</v>
       </c>
       <c r="B121" t="s">
@@ -4099,7 +4114,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+      <c r="A122" s="1" t="s">
         <v>369</v>
       </c>
       <c r="B122" t="s">
@@ -4116,7 +4131,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
         <v>371</v>
       </c>
       <c r="B123" t="s">
@@ -4133,7 +4148,7 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+      <c r="A124" s="1" t="s">
         <v>373</v>
       </c>
       <c r="B124" t="s">
@@ -4150,7 +4165,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+      <c r="A125" s="1" t="s">
         <v>375</v>
       </c>
       <c r="B125" t="s">
@@ -4170,7 +4185,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+      <c r="A126" s="1" t="s">
         <v>378</v>
       </c>
       <c r="B126" t="s">
@@ -4190,7 +4205,7 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+      <c r="A127" s="1" t="s">
         <v>381</v>
       </c>
       <c r="B127" t="s">
@@ -4210,7 +4225,7 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
+      <c r="A128" s="1" t="s">
         <v>384</v>
       </c>
       <c r="B128" t="s">
@@ -4227,7 +4242,7 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+      <c r="A129" s="1" t="s">
         <v>385</v>
       </c>
       <c r="B129" t="s">
@@ -4247,7 +4262,7 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+      <c r="A130" s="1" t="s">
         <v>388</v>
       </c>
       <c r="B130" t="s">
@@ -4267,7 +4282,7 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+      <c r="A131" s="1" t="s">
         <v>391</v>
       </c>
       <c r="B131" t="s">
@@ -4287,7 +4302,7 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+      <c r="A132" s="1" t="s">
         <v>394</v>
       </c>
       <c r="B132" t="s">
@@ -4307,7 +4322,7 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+      <c r="A133" s="1" t="s">
         <v>397</v>
       </c>
       <c r="B133" t="s">
@@ -4327,7 +4342,7 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+      <c r="A134" s="1" t="s">
         <v>400</v>
       </c>
       <c r="B134" t="s">
@@ -4347,7 +4362,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+      <c r="A135" s="1" t="s">
         <v>403</v>
       </c>
       <c r="B135" t="s">
@@ -4367,7 +4382,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+      <c r="A136" s="1" t="s">
         <v>406</v>
       </c>
       <c r="B136" t="s">
@@ -4387,7 +4402,7 @@
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+      <c r="A137" s="1" t="s">
         <v>409</v>
       </c>
       <c r="B137" t="s">
@@ -4407,7 +4422,7 @@
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+      <c r="A138" s="1" t="s">
         <v>412</v>
       </c>
       <c r="B138" t="s">
@@ -4424,7 +4439,7 @@
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+      <c r="A139" s="1" t="s">
         <v>414</v>
       </c>
       <c r="B139" t="s">
@@ -4441,7 +4456,7 @@
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+      <c r="A140" s="1" t="s">
         <v>416</v>
       </c>
       <c r="B140" t="s">
@@ -4461,7 +4476,7 @@
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+      <c r="A141" s="1" t="s">
         <v>420</v>
       </c>
       <c r="B141" t="s">
@@ -4481,7 +4496,7 @@
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+      <c r="A142" s="1" t="s">
         <v>423</v>
       </c>
       <c r="B142" t="s">
@@ -4501,7 +4516,7 @@
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+      <c r="A143" s="1" t="s">
         <v>426</v>
       </c>
       <c r="B143" t="s">
@@ -4521,7 +4536,7 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+      <c r="A144" s="1" t="s">
         <v>429</v>
       </c>
       <c r="B144" t="s">
@@ -4538,7 +4553,7 @@
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+      <c r="A145" s="1" t="s">
         <v>431</v>
       </c>
       <c r="B145" t="s">
@@ -4558,7 +4573,7 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
+      <c r="A146" s="1" t="s">
         <v>434</v>
       </c>
       <c r="B146" t="s">
@@ -4575,7 +4590,7 @@
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
+      <c r="A147" s="1" t="s">
         <v>436</v>
       </c>
       <c r="B147" t="s">
@@ -4592,7 +4607,7 @@
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
+      <c r="A148" s="1" t="s">
         <v>438</v>
       </c>
       <c r="B148" t="s">
@@ -4612,7 +4627,7 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
+      <c r="A149" s="1" t="s">
         <v>441</v>
       </c>
       <c r="B149" t="s">
@@ -4632,7 +4647,7 @@
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
+      <c r="A150" s="1" t="s">
         <v>351</v>
       </c>
       <c r="B150" t="s">
@@ -4649,7 +4664,7 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
+      <c r="A151" s="1" t="s">
         <v>445</v>
       </c>
       <c r="B151" t="s">
@@ -4666,7 +4681,7 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
+      <c r="A152" s="1" t="s">
         <v>447</v>
       </c>
       <c r="B152" t="s">
@@ -4683,7 +4698,7 @@
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A153" t="s">
+      <c r="A153" s="1" t="s">
         <v>449</v>
       </c>
       <c r="D153" t="s">

</xml_diff>